<commit_message>
fix intrus dans admin1
</commit_message>
<xml_diff>
--- a/storage/app/public/input data/caseloads/wca.xlsx
+++ b/storage/app/public/input data/caseloads/wca.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\database\public\uploads\caseloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitednations.sharepoint.com/sites/OCHAROWCA/Information Management/30 DataBase/datas/caseloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6490C-354B-45BA-98C8-3FBE5D2E8374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{89B6490C-354B-45BA-98C8-3FBE5D2E8374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58084C62-2C15-4E78-AA34-F1EA851754E4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="102">
   <si>
     <t>Country</t>
   </si>
@@ -112,13 +120,242 @@
   </si>
   <si>
     <t>SEN</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Democratic Republic of Congo</t>
+  </si>
+  <si>
+    <t>DRC</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Cameroon (Extreme-Nord)</t>
+  </si>
+  <si>
+    <t>Extreme Nord</t>
+  </si>
+  <si>
+    <t>CM04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senegal </t>
+  </si>
+  <si>
+    <t>Agadez</t>
+  </si>
+  <si>
+    <t>Diffa</t>
+  </si>
+  <si>
+    <t>Dosso</t>
+  </si>
+  <si>
+    <t>Maradi</t>
+  </si>
+  <si>
+    <t>Niamey</t>
+  </si>
+  <si>
+    <t>Tahoua</t>
+  </si>
+  <si>
+    <t>Tillaberi</t>
+  </si>
+  <si>
+    <t>Zinder</t>
+  </si>
+  <si>
+    <t>Adamawa</t>
+  </si>
+  <si>
+    <t>Borno</t>
+  </si>
+  <si>
+    <t>Yobe</t>
+  </si>
+  <si>
+    <t>Boucle du Mouhoun</t>
+  </si>
+  <si>
+    <t>Centre-Est</t>
+  </si>
+  <si>
+    <t>Centre-Nord</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Nord</t>
+  </si>
+  <si>
+    <t>Sahel</t>
+  </si>
+  <si>
+    <t>Barh-El-Gazel</t>
+  </si>
+  <si>
+    <t>Batha</t>
+  </si>
+  <si>
+    <t>Borkou</t>
+  </si>
+  <si>
+    <t>Chari-Baguirmi</t>
+  </si>
+  <si>
+    <t>Ennedi Est</t>
+  </si>
+  <si>
+    <t>Ennedi Ouest</t>
+  </si>
+  <si>
+    <t>Guera</t>
+  </si>
+  <si>
+    <t>Hadjer Lamis</t>
+  </si>
+  <si>
+    <t>Kanem</t>
+  </si>
+  <si>
+    <t>Lac</t>
+  </si>
+  <si>
+    <t>Logone Occidental</t>
+  </si>
+  <si>
+    <t>Logone Oriental</t>
+  </si>
+  <si>
+    <t>Mandoul</t>
+  </si>
+  <si>
+    <t>Mayo-Kebbi Est</t>
+  </si>
+  <si>
+    <t>Mayo-Kebbi Ouest</t>
+  </si>
+  <si>
+    <t>Moyen-Chari</t>
+  </si>
+  <si>
+    <t>N'Djamena</t>
+  </si>
+  <si>
+    <t>Ouaddai</t>
+  </si>
+  <si>
+    <t>Salamat</t>
+  </si>
+  <si>
+    <t>Sila</t>
+  </si>
+  <si>
+    <t>Tandjile</t>
+  </si>
+  <si>
+    <t>Tibesti</t>
+  </si>
+  <si>
+    <t>Wadi Fira</t>
+  </si>
+  <si>
+    <t>Bamako</t>
+  </si>
+  <si>
+    <t>ML09</t>
+  </si>
+  <si>
+    <t>Gao</t>
+  </si>
+  <si>
+    <t>ML07</t>
+  </si>
+  <si>
+    <t>Kayes</t>
+  </si>
+  <si>
+    <t>ML01</t>
+  </si>
+  <si>
+    <t>Kidal</t>
+  </si>
+  <si>
+    <t>ML08</t>
+  </si>
+  <si>
+    <t>Koulikouro</t>
+  </si>
+  <si>
+    <t>ML02</t>
+  </si>
+  <si>
+    <t>Mopti</t>
+  </si>
+  <si>
+    <t>ML05</t>
+  </si>
+  <si>
+    <t>Segou</t>
+  </si>
+  <si>
+    <t>ML04</t>
+  </si>
+  <si>
+    <t>Sikasso</t>
+  </si>
+  <si>
+    <t>ML03</t>
+  </si>
+  <si>
+    <t>Tombouctou</t>
+  </si>
+  <si>
+    <t>ML06</t>
+  </si>
+  <si>
+    <t>BF46</t>
+  </si>
+  <si>
+    <t>BF48</t>
+  </si>
+  <si>
+    <t>BF49</t>
+  </si>
+  <si>
+    <t>BF52</t>
+  </si>
+  <si>
+    <t>BF54</t>
+  </si>
+  <si>
+    <t>BF56</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,19 +381,61 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Milliers [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,8 +451,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED10DA4E-D105-481B-ACFC-A68C22FCFC16}" name="Tableau1" displayName="Tableau1" ref="A1:J33" totalsRowShown="0">
-  <autoFilter ref="A1:J33" xr:uid="{3464EA4F-FC43-4D04-8195-39A8D46F9942}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED10DA4E-D105-481B-ACFC-A68C22FCFC16}" name="Tableau1" displayName="Tableau1" ref="A1:J95" totalsRowShown="0">
+  <autoFilter ref="A1:J95" xr:uid="{3464EA4F-FC43-4D04-8195-39A8D46F9942}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Burkina Faso"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{594076F3-52C5-4F4D-87D8-6757CB8DC572}" name="Country"/>
     <tableColumn id="2" xr3:uid="{CBF2065D-E791-43E6-ABC3-D697932CF83D}" name="Country_Iso3"/>
@@ -181,8 +466,8 @@
     <tableColumn id="4" xr3:uid="{996E4742-C7CE-43D3-8D01-74778BF1B7E1}" name="Admin1_pcode"/>
     <tableColumn id="5" xr3:uid="{6FA592D9-4C73-49DE-AF4B-5C9CEAC53494}" name="Total_population"/>
     <tableColumn id="6" xr3:uid="{230C7462-DD32-43CC-9F80-0292F57539E9}" name="People_affected"/>
-    <tableColumn id="7" xr3:uid="{9FB4AA86-862C-4650-9E74-E6F8AB7C5B02}" name="People_in_need"/>
-    <tableColumn id="8" xr3:uid="{6A669401-7064-442C-B28C-63A9FF0888F1}" name="People_targeted"/>
+    <tableColumn id="7" xr3:uid="{9FB4AA86-862C-4650-9E74-E6F8AB7C5B02}" name="People_in_need" dataDxfId="2" dataCellStyle="Milliers [0]"/>
+    <tableColumn id="8" xr3:uid="{6A669401-7064-442C-B28C-63A9FF0888F1}" name="People_targeted" dataDxfId="1" dataCellStyle="Milliers [0]"/>
     <tableColumn id="9" xr3:uid="{025746CC-F599-4DAC-A9D7-4C294979CDD2}" name="People_reached"/>
     <tableColumn id="10" xr3:uid="{FEA66360-662B-40D7-A391-58CB1ADA1AFF}" name="Date" dataDxfId="0"/>
   </tableColumns>
@@ -453,17 +738,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
@@ -518,10 +803,10 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>1551147.4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>833153.16850390995</v>
       </c>
       <c r="I2" t="s">
@@ -531,7 +816,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -544,10 +829,10 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>2300000</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>1800000</v>
       </c>
       <c r="I3" t="s">
@@ -557,7 +842,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -570,10 +855,10 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>1479172</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>624090</v>
       </c>
       <c r="I4" t="s">
@@ -583,7 +868,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -596,10 +881,10 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>181861</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>181861</v>
       </c>
       <c r="I5" t="s">
@@ -609,7 +894,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -622,10 +907,10 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>2500000</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>1000000</v>
       </c>
       <c r="I6" t="s">
@@ -635,7 +920,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -648,10 +933,10 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>468000</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>377000</v>
       </c>
       <c r="I7" t="s">
@@ -661,7 +946,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -674,10 +959,10 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>2000000</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>1500000</v>
       </c>
       <c r="I8" t="s">
@@ -687,7 +972,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -700,10 +985,10 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>7000000</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>3900000</v>
       </c>
       <c r="I9" t="s">
@@ -713,7 +998,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -726,10 +1011,10 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>620000</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>353000</v>
       </c>
       <c r="I10" t="s">
@@ -752,10 +1037,10 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>860625</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>477872</v>
       </c>
       <c r="I11" t="s">
@@ -765,7 +1050,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -778,10 +1063,10 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>4400000</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>1900000</v>
       </c>
       <c r="I12" t="s">
@@ -791,7 +1076,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -804,10 +1089,10 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>1555274.2056874</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>734000</v>
       </c>
       <c r="I13" t="s">
@@ -817,7 +1102,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -830,10 +1115,10 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>3700000</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>1360000</v>
       </c>
       <c r="I14" t="s">
@@ -843,7 +1128,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -856,10 +1141,10 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>539000</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>416000</v>
       </c>
       <c r="I15" t="s">
@@ -869,7 +1154,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -882,10 +1167,10 @@
       <c r="D16" t="s">
         <v>18</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>1900000</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>1500000</v>
       </c>
       <c r="I16" t="s">
@@ -895,7 +1180,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -908,10 +1193,10 @@
       <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>8500000</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>6900000</v>
       </c>
       <c r="I17" t="s">
@@ -921,7 +1206,7 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -934,10 +1219,10 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>881000</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>379000</v>
       </c>
       <c r="I18" t="s">
@@ -960,10 +1245,10 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>954000</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>702000</v>
       </c>
       <c r="I19" t="s">
@@ -973,7 +1258,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -986,10 +1271,10 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>4432875.0734043997</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>1882276.0400107</v>
       </c>
       <c r="I20" t="s">
@@ -999,7 +1284,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1012,10 +1297,10 @@
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>2074959.7559215</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>832728.80515269004</v>
       </c>
       <c r="I21" t="s">
@@ -1025,7 +1310,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1038,10 +1323,10 @@
       <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>4100000</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>1560000</v>
       </c>
       <c r="I22" t="s">
@@ -1051,7 +1336,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1064,10 +1349,10 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>2300000</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>1800000</v>
       </c>
       <c r="I23" t="s">
@@ -1077,7 +1362,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1090,10 +1375,10 @@
       <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>7700000</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>6100000</v>
       </c>
       <c r="I24" t="s">
@@ -1103,7 +1388,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1116,10 +1401,10 @@
       <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>814000</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>340000</v>
       </c>
       <c r="I25" t="s">
@@ -1142,10 +1427,10 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>1475690</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>1251427</v>
       </c>
       <c r="I26" t="s">
@@ -1155,7 +1440,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1168,10 +1453,10 @@
       <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>1900000</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>881550</v>
       </c>
       <c r="I27" t="s">
@@ -1181,7 +1466,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1194,10 +1479,10 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>4300000</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>2000000</v>
       </c>
       <c r="I28" t="s">
@@ -1207,7 +1492,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1220,10 +1505,10 @@
       <c r="D29" t="s">
         <v>18</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>3900000</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>3000000</v>
       </c>
       <c r="I29" t="s">
@@ -1233,7 +1518,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1246,10 +1531,10 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>0</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>0</v>
       </c>
       <c r="I30" t="s">
@@ -1259,7 +1544,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1272,10 +1557,10 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="3">
         <v>2300000</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>1600000</v>
       </c>
       <c r="I31" t="s">
@@ -1285,7 +1570,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1298,10 +1583,10 @@
       <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>7100000</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>6200000</v>
       </c>
       <c r="I32" t="s">
@@ -1311,7 +1596,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1324,10 +1609,10 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>0</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>0</v>
       </c>
       <c r="I33" t="s">
@@ -1335,6 +1620,1282 @@
       </c>
       <c r="J33" s="1">
         <v>43767</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2928111</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2104401</v>
+      </c>
+      <c r="I34">
+        <v>1800000</v>
+      </c>
+      <c r="J34" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="3">
+        <v>6200000</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3400000</v>
+      </c>
+      <c r="I35">
+        <v>2200000</v>
+      </c>
+      <c r="J35" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="3">
+        <v>2600000</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1800000</v>
+      </c>
+      <c r="I36">
+        <v>1250000</v>
+      </c>
+      <c r="J36" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6400000</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3800000</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="3">
+        <v>25600000</v>
+      </c>
+      <c r="H38" s="3">
+        <v>9200000</v>
+      </c>
+      <c r="I38">
+        <v>4000000</v>
+      </c>
+      <c r="J38" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="3">
+        <v>6800000</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5500000</v>
+      </c>
+      <c r="I39">
+        <v>888370</v>
+      </c>
+      <c r="J39" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="3">
+        <v>3700000</v>
+      </c>
+      <c r="H40" s="3">
+        <v>2200000</v>
+      </c>
+      <c r="I40">
+        <v>594608</v>
+      </c>
+      <c r="J40" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="3">
+        <v>10600000</v>
+      </c>
+      <c r="H41" s="3">
+        <v>7800000</v>
+      </c>
+      <c r="I41">
+        <v>2600000</v>
+      </c>
+      <c r="J41" s="1">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1200266.79</v>
+      </c>
+      <c r="H42" s="3">
+        <v>950635</v>
+      </c>
+      <c r="J42" s="1">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="3">
+        <v>101375</v>
+      </c>
+      <c r="H45" s="3">
+        <v>166203</v>
+      </c>
+      <c r="J45" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="3">
+        <v>292139</v>
+      </c>
+      <c r="H46" s="3">
+        <v>368645</v>
+      </c>
+      <c r="J46" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="3">
+        <v>468565</v>
+      </c>
+      <c r="H47" s="3">
+        <v>468565</v>
+      </c>
+      <c r="J47" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G48" s="3">
+        <v>703807</v>
+      </c>
+      <c r="H48" s="3">
+        <v>703807</v>
+      </c>
+      <c r="J48" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="3">
+        <v>30647</v>
+      </c>
+      <c r="H49" s="3">
+        <v>75220</v>
+      </c>
+      <c r="J49" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="3">
+        <v>816928</v>
+      </c>
+      <c r="H50" s="3">
+        <v>816928</v>
+      </c>
+      <c r="J50" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51" s="3">
+        <v>529795</v>
+      </c>
+      <c r="H51" s="3">
+        <v>529795</v>
+      </c>
+      <c r="J51" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="3">
+        <v>878403</v>
+      </c>
+      <c r="H52" s="3">
+        <v>878403</v>
+      </c>
+      <c r="J52" s="1">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G53" s="3">
+        <v>2230000</v>
+      </c>
+      <c r="H53" s="3">
+        <v>1443000</v>
+      </c>
+      <c r="J53" s="1">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="3">
+        <v>3890000</v>
+      </c>
+      <c r="H54" s="3">
+        <v>3295000</v>
+      </c>
+      <c r="J54" s="1">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G55" s="3">
+        <v>2581000</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1743000</v>
+      </c>
+      <c r="J55" s="1">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" t="s">
+        <v>96</v>
+      </c>
+      <c r="G56" s="3">
+        <v>441204.94795031624</v>
+      </c>
+      <c r="H56" s="3">
+        <v>325305.75405525905</v>
+      </c>
+      <c r="J56" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" t="s">
+        <v>97</v>
+      </c>
+      <c r="G57" s="3">
+        <v>210665.58265954713</v>
+      </c>
+      <c r="H57" s="3">
+        <v>200960.90136715423</v>
+      </c>
+      <c r="J57" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G58" s="3">
+        <v>907915.77231944352</v>
+      </c>
+      <c r="H58" s="3">
+        <v>812392.76</v>
+      </c>
+      <c r="J58" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" s="3">
+        <v>608279.9310292335</v>
+      </c>
+      <c r="H59" s="3">
+        <v>446428.44738497975</v>
+      </c>
+      <c r="J59" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="3">
+        <v>544466.80000000005</v>
+      </c>
+      <c r="H60" s="3">
+        <v>412054.51049999997</v>
+      </c>
+      <c r="J60" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" t="s">
+        <v>101</v>
+      </c>
+      <c r="G61" s="3">
+        <v>821239.99341135425</v>
+      </c>
+      <c r="H61" s="3">
+        <v>722867.76958658011</v>
+      </c>
+      <c r="J61" s="1">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" s="3">
+        <v>149407</v>
+      </c>
+      <c r="H62" s="3">
+        <v>129089</v>
+      </c>
+      <c r="J62" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" s="3">
+        <v>234294</v>
+      </c>
+      <c r="H63" s="3">
+        <v>213856</v>
+      </c>
+      <c r="J63" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="G64" s="3">
+        <v>75614</v>
+      </c>
+      <c r="H64" s="3">
+        <v>35808</v>
+      </c>
+      <c r="J64" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" s="3">
+        <v>143076</v>
+      </c>
+      <c r="H65" s="3">
+        <v>23519</v>
+      </c>
+      <c r="J65" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" s="3">
+        <v>96818</v>
+      </c>
+      <c r="H66" s="3">
+        <v>70204</v>
+      </c>
+      <c r="J66" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+      <c r="G67" s="3">
+        <v>33766</v>
+      </c>
+      <c r="H67" s="3">
+        <v>8244</v>
+      </c>
+      <c r="J67" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>61</v>
+      </c>
+      <c r="G68" s="3">
+        <v>215307</v>
+      </c>
+      <c r="H68" s="3">
+        <v>192843</v>
+      </c>
+      <c r="J68" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="3">
+        <v>275031</v>
+      </c>
+      <c r="H69" s="3">
+        <v>101178</v>
+      </c>
+      <c r="J69" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="G70" s="3">
+        <v>240029</v>
+      </c>
+      <c r="H70" s="3">
+        <v>230531</v>
+      </c>
+      <c r="J70" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>64</v>
+      </c>
+      <c r="G71" s="3">
+        <v>389875</v>
+      </c>
+      <c r="H71" s="3">
+        <v>378523</v>
+      </c>
+      <c r="J71" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>65</v>
+      </c>
+      <c r="G72" s="3">
+        <v>273633</v>
+      </c>
+      <c r="H72" s="3">
+        <v>85783</v>
+      </c>
+      <c r="J72" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>66</v>
+      </c>
+      <c r="G73" s="3">
+        <v>417257</v>
+      </c>
+      <c r="H73" s="3">
+        <v>367650</v>
+      </c>
+      <c r="J73" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>67</v>
+      </c>
+      <c r="G74" s="3">
+        <v>207668</v>
+      </c>
+      <c r="H74" s="3">
+        <v>207668</v>
+      </c>
+      <c r="J74" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75" s="3">
+        <v>236494</v>
+      </c>
+      <c r="H75" s="3">
+        <v>61467</v>
+      </c>
+      <c r="J75" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G76" s="3">
+        <v>129239</v>
+      </c>
+      <c r="H76" s="3">
+        <v>22689</v>
+      </c>
+      <c r="J76" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" t="s">
+        <v>70</v>
+      </c>
+      <c r="G77" s="3">
+        <v>220232</v>
+      </c>
+      <c r="H77" s="3">
+        <v>220232</v>
+      </c>
+      <c r="J77" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>71</v>
+      </c>
+      <c r="G78" s="3">
+        <v>503388</v>
+      </c>
+      <c r="H78" s="3">
+        <v>271338</v>
+      </c>
+      <c r="J78" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="G79" s="3">
+        <v>487600</v>
+      </c>
+      <c r="H79" s="3">
+        <v>437152</v>
+      </c>
+      <c r="J79" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>73</v>
+      </c>
+      <c r="G80" s="3">
+        <v>160711</v>
+      </c>
+      <c r="H80" s="3">
+        <v>131304</v>
+      </c>
+      <c r="J80" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" t="s">
+        <v>74</v>
+      </c>
+      <c r="G81" s="3">
+        <v>280686</v>
+      </c>
+      <c r="H81" s="3">
+        <v>230057</v>
+      </c>
+      <c r="J81" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" t="s">
+        <v>75</v>
+      </c>
+      <c r="G82" s="3">
+        <v>221941</v>
+      </c>
+      <c r="H82" s="3">
+        <v>50155</v>
+      </c>
+      <c r="J82" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" t="s">
+        <v>76</v>
+      </c>
+      <c r="G83" s="3">
+        <v>20418</v>
+      </c>
+      <c r="H83" s="3">
+        <v>10121</v>
+      </c>
+      <c r="J83" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" t="s">
+        <v>77</v>
+      </c>
+      <c r="G84" s="3">
+        <v>484166</v>
+      </c>
+      <c r="H84" s="3">
+        <v>484166</v>
+      </c>
+      <c r="J84" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D85" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="3">
+        <v>345156.00000000006</v>
+      </c>
+      <c r="H85" s="3">
+        <v>258867</v>
+      </c>
+      <c r="J85" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" t="s">
+        <v>80</v>
+      </c>
+      <c r="D86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G86" s="3">
+        <v>697639.17981515499</v>
+      </c>
+      <c r="H86" s="3">
+        <v>570618.19385212369</v>
+      </c>
+      <c r="J86" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" t="s">
+        <v>82</v>
+      </c>
+      <c r="D87" t="s">
+        <v>83</v>
+      </c>
+      <c r="G87" s="3">
+        <v>443658.70589092915</v>
+      </c>
+      <c r="H87" s="3">
+        <v>350499.51471274334</v>
+      </c>
+      <c r="J87" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" t="s">
+        <v>84</v>
+      </c>
+      <c r="D88" t="s">
+        <v>85</v>
+      </c>
+      <c r="G88" s="3">
+        <v>79151.403774561011</v>
+      </c>
+      <c r="H88" s="3">
+        <v>51948.419291003331</v>
+      </c>
+      <c r="J88" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" t="s">
+        <v>87</v>
+      </c>
+      <c r="G89" s="3">
+        <v>295615.90207045397</v>
+      </c>
+      <c r="H89" s="3">
+        <v>225123.47165636317</v>
+      </c>
+      <c r="J89" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" t="s">
+        <v>89</v>
+      </c>
+      <c r="G90" s="3">
+        <v>1674208.8003478548</v>
+      </c>
+      <c r="H90" s="3">
+        <v>1335324.0792901064</v>
+      </c>
+      <c r="J90" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" t="s">
+        <v>90</v>
+      </c>
+      <c r="D91" t="s">
+        <v>91</v>
+      </c>
+      <c r="G91" s="3">
+        <v>1228524.6507884786</v>
+      </c>
+      <c r="H91" s="3">
+        <v>1035037.6175668903</v>
+      </c>
+      <c r="J91" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D92" t="s">
+        <v>93</v>
+      </c>
+      <c r="G92" s="3">
+        <v>145111.14614263049</v>
+      </c>
+      <c r="H92" s="3">
+        <v>111082.31691410438</v>
+      </c>
+      <c r="J92" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" t="s">
+        <v>95</v>
+      </c>
+      <c r="G93" s="3">
+        <v>1008202.9918570882</v>
+      </c>
+      <c r="H93" s="3">
+        <v>806562.39348567056</v>
+      </c>
+      <c r="J93" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+      <c r="G94" s="3">
+        <v>2800000</v>
+      </c>
+      <c r="H94" s="3">
+        <v>1840000</v>
+      </c>
+      <c r="J94" s="1">
+        <v>44179</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" s="3">
+        <v>19600000</v>
+      </c>
+      <c r="H95" s="3">
+        <v>9600000</v>
+      </c>
+      <c r="J95" s="1">
+        <v>44224</v>
       </c>
     </row>
   </sheetData>
@@ -1343,4 +2904,272 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D56D188CBA27BF43BA16AB0991F8810A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d74f8ed3820e849c6c24bebf382cead">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d04cdad-faad-4bbc-9725-fbca26071bed" xmlns:ns3="d4bd7185-3ccc-47d5-be69-542fd420c7c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="92b3107f17917cdf1896d29dfba996e5" ns2:_="" ns3:_="">
+    <xsd:import namespace="2d04cdad-faad-4bbc-9725-fbca26071bed"/>
+    <xsd:import namespace="d4bd7185-3ccc-47d5-be69-542fd420c7c8"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2d04cdad-faad-4bbc-9725-fbca26071bed" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d4bd7185-3ccc-47d5-be69-542fd420c7c8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="4" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="3" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349C11E4-6325-4393-B8C1-38F3019EC890}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2d04cdad-faad-4bbc-9725-fbca26071bed"/>
+    <ds:schemaRef ds:uri="d4bd7185-3ccc-47d5-be69-542fd420c7c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511CA8EF-A5B7-44F6-9EAB-5A51880E4BA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3984A634-41E9-40B9-843B-B3915C32AE6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>